<commit_message>
toast, tile, purchasing (both apps) - all ready for packaging
</commit_message>
<xml_diff>
--- a/testplan.xlsx
+++ b/testplan.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>Название</t>
   </si>
   <si>
-    <t>Windows</t>
-  </si>
-  <si>
     <t>SmartTile со стр. настроек</t>
   </si>
   <si>
@@ -47,20 +44,29 @@
     <t>Вирт. машина</t>
   </si>
   <si>
-    <t>WP</t>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
     <t>Стандартная плитка</t>
+  </si>
+  <si>
+    <t>Windows + файл</t>
+  </si>
+  <si>
+    <t>WP + файл</t>
+  </si>
+  <si>
+    <t>Windows без файла</t>
+  </si>
+  <si>
+    <t>WP без файла</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,8 +84,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,6 +103,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -116,11 +136,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -128,12 +149,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="20% — акцент1" xfId="2" builtinId="30"/>
     <cellStyle name="Контрольная ячейка" xfId="1" builtinId="23"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -157,13 +188,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Таблица3" displayName="Таблица3" ref="A1:D24" totalsRowShown="0">
-  <autoFilter ref="A1:D24"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Таблица3" displayName="Таблица3" ref="A1:F24" totalsRowShown="0">
+  <autoFilter ref="A1:F24"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Название"/>
-    <tableColumn id="2" name="Windows" dataDxfId="2"/>
-    <tableColumn id="3" name="WP" dataDxfId="1"/>
-    <tableColumn id="4" name="Вирт. машина" dataDxfId="0"/>
+    <tableColumn id="2" name="Windows + файл" dataDxfId="4"/>
+    <tableColumn id="3" name="WP + файл" dataDxfId="3"/>
+    <tableColumn id="4" name="Вирт. машина" dataDxfId="2"/>
+    <tableColumn id="5" name="Windows без файла" dataDxfId="1"/>
+    <tableColumn id="6" name="WP без файла" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -466,170 +499,243 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="2"/>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>